<commit_message>
Created the DtaProvider Util for the Excel Data that is used in the Createjob api test
Added the LoginAPIExcelDataDrivenTest and
CreateJobAPIExcelDataDrivenTest in testng-datadriven.xml file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/PhoenixTestData.xlsx
+++ b/src/test/resources/testData/PhoenixTestData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SDET with Jatin\Java Module\PhoenixTestAutomationFramework\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F014B3D4-7664-4903-BD2F-F84853C1A959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E17A3E-2A20-4AB0-A7FB-374EFAEFA8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="477" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateJobTestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="56">
   <si>
     <t>username</t>
   </si>
@@ -43,19 +44,174 @@
   </si>
   <si>
     <t>iamqc</t>
+  </si>
+  <si>
+    <t>mst_service_location_id</t>
+  </si>
+  <si>
+    <t>mst_platform_id</t>
+  </si>
+  <si>
+    <t>mst_warrenty_status_id</t>
+  </si>
+  <si>
+    <t>mst_oem_id</t>
+  </si>
+  <si>
+    <t>customer__first_name</t>
+  </si>
+  <si>
+    <t>customer__last_name</t>
+  </si>
+  <si>
+    <t>customer__mobile_number</t>
+  </si>
+  <si>
+    <t>customer__mobile_number_alt</t>
+  </si>
+  <si>
+    <t>customer__email_id</t>
+  </si>
+  <si>
+    <t>customer__email_id_alt</t>
+  </si>
+  <si>
+    <t>customer_address__flat_number</t>
+  </si>
+  <si>
+    <t>customer_address__apartment_name</t>
+  </si>
+  <si>
+    <t>customer_address__street_name</t>
+  </si>
+  <si>
+    <t>customer_address__landmark</t>
+  </si>
+  <si>
+    <t>customer_address__area</t>
+  </si>
+  <si>
+    <t>customer_address__pincode</t>
+  </si>
+  <si>
+    <t>customer_address__country</t>
+  </si>
+  <si>
+    <t>customer_address__state</t>
+  </si>
+  <si>
+    <t>customer_product__dop</t>
+  </si>
+  <si>
+    <t>customer_product__serial_number</t>
+  </si>
+  <si>
+    <t>customer_product__imei1</t>
+  </si>
+  <si>
+    <t>customer_product__imei2</t>
+  </si>
+  <si>
+    <t>customer_product__popurl</t>
+  </si>
+  <si>
+    <t>customer_product__product_id</t>
+  </si>
+  <si>
+    <t>customer_product__mst_model_id</t>
+  </si>
+  <si>
+    <t>problems__id</t>
+  </si>
+  <si>
+    <t>problems__remark</t>
+  </si>
+  <si>
+    <t>Madelyn</t>
+  </si>
+  <si>
+    <t>Bartell</t>
+  </si>
+  <si>
+    <t>316-628-5442</t>
+  </si>
+  <si>
+    <t>Willie43@yahoo.com</t>
+  </si>
+  <si>
+    <t>Brigade Gateway</t>
+  </si>
+  <si>
+    <t>Dr. Rajkumar Road</t>
+  </si>
+  <si>
+    <t>Orion Mall</t>
+  </si>
+  <si>
+    <t>Rajajinagar</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>2025-08-24T18:30:00.000Z</t>
+  </si>
+  <si>
+    <t>Smartphone is running slow</t>
+  </si>
+  <si>
+    <t>Chetan</t>
+  </si>
+  <si>
+    <t>Ajinkya</t>
+  </si>
+  <si>
+    <t>Jatin</t>
+  </si>
+  <si>
+    <t>Ritu</t>
+  </si>
+  <si>
+    <t>Adi</t>
+  </si>
+  <si>
+    <t>47894547389246</t>
+  </si>
+  <si>
+    <t>36784938340803</t>
+  </si>
+  <si>
+    <t>79394893208403</t>
+  </si>
+  <si>
+    <t>48349583224463</t>
+  </si>
+  <si>
+    <t>38290923182914</t>
+  </si>
+  <si>
+    <t>98272363473274</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,14 +231,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{76D53EC6-8AB7-4744-A12D-DC6826660544}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -362,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -415,4 +575,604 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCA7C4E-3C5E-40ED-A321-644700D31CF8}">
+  <dimension ref="A1:AA7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1">
+        <v>302</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="1">
+        <v>560055</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1">
+        <v>302</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="1">
+        <v>560055</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1">
+        <v>302</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="1">
+        <v>560055</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1">
+        <v>302</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="1">
+        <v>560055</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1">
+        <v>302</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="1">
+        <v>560055</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1">
+        <v>302</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P7" s="1">
+        <v>560055</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>